<commit_message>
Update the column headers for the specify check to be clearer.
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\GitHub\high-frequency-checks\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>consent_value</t>
-  </si>
-  <si>
-    <t>specify_variable</t>
   </si>
   <si>
     <t>surveystart</t>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>multiplier</t>
-  </si>
-  <si>
-    <t>other_variable</t>
   </si>
   <si>
     <t>Survey ID</t>
@@ -188,6 +182,12 @@
   </si>
   <si>
     <t>Geographic Cluster</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>parent</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,65 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1062,17 +1120,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>specify_variable</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
+            <a:t>child</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the names of the specify other variables.</a:t>
+            <a:t>This column specifies the names of the specify other variables containing the actual text of the response specified.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1508,17 +1563,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>other_variable</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
+            <a:t>parent</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the names of the original select_one or select_multiple questions containing the other choice options.</a:t>
+            <a:t>This column specifies the names of the original select_one or select_multiple questions containing an "other" choice option.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -9140,7 +9192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -9153,7 +9205,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="26"/>
@@ -9165,56 +9217,56 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10"/>
@@ -9226,42 +9278,42 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="10"/>
@@ -9273,42 +9325,42 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -9320,21 +9372,21 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="10"/>
@@ -9369,24 +9421,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -9449,12 +9501,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>$A1="specify_variable"</formula>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$A1="child"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9481,19 +9533,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -9516,12 +9568,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9545,13 +9597,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -9574,12 +9626,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9600,22 +9652,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -9823,12 +9875,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9849,7 +9901,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -9875,16 +9927,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9892,12 +9944,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9921,10 +9973,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -9935,12 +9987,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9967,10 +10019,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9978,12 +10030,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10007,10 +10059,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -10045,12 +10097,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10074,13 +10126,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10097,12 +10149,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10126,16 +10178,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -10163,12 +10215,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10192,7 +10244,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -10720,12 +10772,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10761,10 +10813,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -11234,12 +11286,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update input sheet, do-file, and import command to incoporate program.
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\GitHub\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -25,14 +25,15 @@
     <sheet name="10. dates" sheetId="10" r:id="rId11"/>
     <sheet name="11. outliers" sheetId="11" r:id="rId12"/>
     <sheet name="enumdb" sheetId="13" r:id="rId13"/>
-    <sheet name="researchdb" sheetId="14" r:id="rId14"/>
+    <sheet name="research oneway" sheetId="16" r:id="rId14"/>
+    <sheet name="research twoway" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>variable</t>
   </si>
@@ -80,9 +81,6 @@
   </si>
   <si>
     <t>exclude_variable</t>
-  </si>
-  <si>
-    <t>coming soon</t>
   </si>
   <si>
     <t>complete_value</t>
@@ -188,6 +186,12 @@
   </si>
   <si>
     <t>parent</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>by</t>
   </si>
 </sst>
 </file>
@@ -490,7 +494,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="34">
     <dxf>
       <border>
         <left style="thin">
@@ -548,6 +552,93 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -3791,6 +3882,1133 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E1BD9C0-3302-4B5D-8CA3-6304689AEA06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="47625"/>
+          <a:ext cx="3648075" cy="1628775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Research</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> Dashboard: One-Way Summary</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Display one-way summaries of important research variables to monitor responses frequecies</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>/distributions.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> command produces a spreadsheet of one-way variable summaries. It can be used to monitor response frequencies/distributions for key variables and help identify any threats to research validity.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97146BD2-7D91-4400-8417-14DBBF0976A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="1762125"/>
+          <a:ext cx="3667125" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the list of variables which will be used to create one-way summaries</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A4A004E-57D7-4664-8277-94BF865E1756}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="2657475"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>type</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the name of variables whose rates of missing values are output per enumerator</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90BE6852-E937-4805-8D84-AF1EBFCBAF51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8439150" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99456BCB-9A07-4EA3-B43D-5E6707D9FC42}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED684BB-CA02-486D-B3A5-87458AE4D1C2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E19F774-B7DC-43FD-806D-25281EF01B95}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948A900B-462D-4465-88B1-F85FFA112D04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="3371850"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>notes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4F39785-3E5C-4EDB-8458-11C2D94E9F1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="47625"/>
+          <a:ext cx="3648075" cy="1628775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Research</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> Dashboard: Two-Way Summaries</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Display two-way summaries of important research variables to monitor responses frequecies</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>/distributions.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> command produces a spreadsheet of two-way variable summaries. It can be used to monitor response frequencies/distributions for key variables and help identify any threats to research validity.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDA3C4F-A6F1-42FD-A48B-6EAEECC7B6AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="1762125"/>
+          <a:ext cx="3667125" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the list of variables which will be used to create one-way summaries</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DE122CE-7AC0-4A85-BFA9-EA87EF8C5719}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="2657475"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>type</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the name of variables whose rates of missing values are output per enumerator</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1952D21-D5C5-496F-9B18-C4901FBC371F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3352800"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>by</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0476C836-6DBF-48DA-9F5A-6F66818D7249}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9820275" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{274FCDEC-E4BF-4431-97B8-0BB21899155A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0405F252-A2B3-478F-B537-429EC583D831}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF7C885-F52A-4297-A854-B8FD11B8B8A0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D09948A9-C422-4393-A195-3DB0DC828251}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5591175" y="4048125"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>notes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9205,7 +10423,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="26"/>
@@ -9217,56 +10435,56 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10"/>
@@ -9278,42 +10496,42 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="10"/>
@@ -9325,42 +10543,42 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -9372,21 +10590,21 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="10"/>
@@ -9421,7 +10639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -9429,13 +10647,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -9501,12 +10719,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>$A1="child"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9536,13 +10754,13 @@
         <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>10</v>
@@ -9568,12 +10786,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9597,10 +10815,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -9626,12 +10844,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9645,7 +10863,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -9875,12 +11093,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9891,21 +11109,379 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3"/>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3"/>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="3"/>
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="3"/>
+      <c r="C59" s="4"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="3"/>
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="3"/>
+      <c r="C70" s="4"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="3"/>
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="3"/>
+      <c r="C81" s="4"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$A1="variable"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="D70" s="4"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="D81" s="4"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:D1">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>$A$1="variable"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:D1048576">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9927,13 +11503,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -9944,12 +11520,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9973,7 +11549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
@@ -9987,12 +11563,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="30" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10019,7 +11595,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -10030,12 +11606,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10059,7 +11635,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
@@ -10097,12 +11673,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10126,10 +11702,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -10149,12 +11725,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10181,10 +11757,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -10215,12 +11791,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10772,12 +12348,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10813,7 +12389,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>10</v>
@@ -11286,12 +12862,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
includes tab for text audit and boxes for comments and text audits
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\GitHub\high-frequency-checks\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="enumdb" sheetId="13" r:id="rId13"/>
     <sheet name="research oneway" sheetId="16" r:id="rId14"/>
     <sheet name="research twoway" sheetId="17" r:id="rId15"/>
+    <sheet name="text audit" sheetId="19" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>variable</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t>soft_min</t>
-  </si>
-  <si>
-    <t>soft_max</t>
   </si>
   <si>
     <t>hard_min</t>
@@ -193,6 +191,30 @@
   <si>
     <t>by</t>
   </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>sofft_max</t>
+  </si>
+  <si>
+    <t>Text Audit File (opt.)</t>
+  </si>
+  <si>
+    <t>Text Audit</t>
+  </si>
+  <si>
+    <t>group_name</t>
+  </si>
+  <si>
+    <t>Field Comment</t>
+  </si>
+  <si>
+    <t>Replacements Log (opt.)</t>
+  </si>
 </sst>
 </file>
 
@@ -236,12 +258,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.24994659260841701"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -251,16 +273,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -320,13 +342,13 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -335,10 +357,10 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -347,13 +369,13 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -365,24 +387,24 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -400,36 +422,75 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -472,6 +533,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -494,20 +570,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="35">
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -543,6 +619,42 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -556,16 +668,92 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -601,29 +789,18 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -643,16 +820,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -672,16 +849,34 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -701,16 +896,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -730,16 +925,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -759,16 +954,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -788,16 +983,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -817,16 +1012,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -846,16 +1041,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -875,16 +1070,16 @@
     <dxf>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
+          <color theme="0" tint="-0.49995422223578601"/>
         </bottom>
       </border>
     </dxf>
@@ -2501,13 +2696,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2591,13 +2786,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -2672,13 +2867,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -2750,13 +2945,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -2844,13 +3039,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2922,13 +3117,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -2946,7 +3141,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="361950"/>
+          <a:off x="11649075" y="361950"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -5221,17 +5416,622 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DC2198-C445-4818-9BD5-256B3A518007}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="47626"/>
+          <a:ext cx="3648075" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Text Audits</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Display time (in</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> seconds) spent on each field.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> command produces a spreadsheet of average time spent on each field and group by enumerator</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D5AABD-5DE5-46C6-9F00-821662E28DB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="1819275"/>
+          <a:ext cx="3667125" cy="638175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the name of variables to include for group. Use * for all variables in the group</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E7E9586-5EA4-499A-AF89-F046564EEFB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="1143000"/>
+          <a:ext cx="3657600" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>group_name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies time duration variables. Mean duration per enumerator is output for these variables.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B97EBB5-A753-4218-9CBB-0000619EFAB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5562600" y="2571749"/>
+          <a:ext cx="3667125" cy="819151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>exclude_variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies variables to exclude from group. This column be used to exclude variable when wild cards are used</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>in the variable column </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{955FF48E-8E20-44B1-9EDE-376839A5FD07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9820275" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D78D2CB-AE91-4EBC-A96E-1AEB1E0DCCEA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51379E45-9E4C-48D9-BB97-35F8C40568EA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD6E7E3-2331-41D5-8639-875805325772}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAB8F38A-13C0-4591-BC1E-E542D2401DE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3476625"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -5315,13 +6115,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -5396,13 +6196,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -5474,16 +6274,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5498,7 +6298,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6972300" y="4000500"/>
+          <a:off x="8305800" y="4562475"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5568,16 +6368,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5592,7 +6392,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6972300" y="4695825"/>
+          <a:off x="8324850" y="5286375"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5646,13 +6446,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -5670,7 +6470,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11191875" y="314325"/>
+          <a:off x="11763375" y="314325"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -5839,13 +6639,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
@@ -5908,6 +6708,83 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
             <a:t>This column specifies a minimum non-missing percentage for each interview. Any interview that falls below this threshold will be flagged as incomplete and included in the output.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D2185D-E54E-4253-B3B9-F81BF0C3436F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8324850" y="3848100"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>if_condition</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional in condition for this check. consent == 1</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -9433,13 +10310,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -9544,13 +10421,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -9625,13 +10502,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -9703,13 +10580,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -9797,13 +10674,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -9875,13 +10752,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -9952,13 +10829,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -10046,13 +10923,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -10124,13 +11001,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -10148,7 +11025,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13954125" y="581025"/>
+          <a:off x="16544925" y="581025"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -10615,10 +11492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10629,209 +11506,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>42</v>
+      <c r="A1" s="33" t="s">
+        <v>41</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="11"/>
+    <row r="11" spans="1:3">
+      <c r="A11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="17" t="s">
-        <v>32</v>
+      <c r="A12" s="32" t="s">
+        <v>55</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
-        <v>33</v>
+      <c r="B12" s="30"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="17" t="s">
+        <v>31</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="30"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
-        <v>39</v>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A22" s="21"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="17" t="s">
+        <v>33</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="11"/>
+    <row r="25" spans="1:3">
+      <c r="A25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
+      <c r="B31" s="23"/>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="8"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="8"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10847,23 +11752,23 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -10874,6 +11779,7 @@
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="5" spans="1:4">
@@ -10926,12 +11832,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>$A1="child"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10944,8 +11850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -10958,26 +11864,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:7">
@@ -10993,13 +11899,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="A1:G1 A3:G1048576 A2:B2 D2:G2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11009,55 +11920,78 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="27.5703125" style="25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="27" customFormat="1">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>24</v>
+      <c r="B1" s="26" t="s">
+        <v>52</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
+      <c r="C1" s="26" t="s">
+        <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
+      <c r="D1" s="26" t="s">
+        <v>20</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+      <c r="E1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" s="27" customFormat="1">
+      <c r="A2" s="26"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" s="27" customFormat="1">
+      <c r="A3" s="26"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:6" s="27" customFormat="1">
+      <c r="A4" s="26"/>
+      <c r="C4" s="6"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" s="27" customFormat="1">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="27"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="7" priority="2">
+  <conditionalFormatting sqref="A1:E1">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="A1:E1 A3:E1048576 A2:C2 E2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11070,35 +12004,35 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
@@ -11112,15 +12046,18 @@
     <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3"/>
@@ -11143,8 +12080,10 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="3"/>
       <c r="F15" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3"/>
@@ -11167,8 +12106,10 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
       <c r="F26" s="4"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3"/>
@@ -11191,8 +12132,10 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="3"/>
       <c r="F37" s="4"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="3"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3"/>
@@ -11215,8 +12158,10 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="3"/>
       <c r="F48" s="4"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3"/>
@@ -11239,8 +12184,10 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="3"/>
       <c r="F59" s="4"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="3"/>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="3"/>
@@ -11263,8 +12210,10 @@
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="3"/>
       <c r="F70" s="4"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="3"/>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="3"/>
@@ -11287,11 +12236,12 @@
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="3"/>
       <c r="F81" s="4"/>
     </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="3"/>
+    </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -11300,12 +12250,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11318,8 +12268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11329,10 +12279,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -11490,12 +12440,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11508,8 +12458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11519,16 +12469,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>52</v>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
+      <c r="A2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
     </row>
@@ -11678,13 +12629,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$A$1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:D1 A3:D1048576 D2">
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C2">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A2&lt;&gt;"", $B2&lt;&gt;"", $C2&lt;&gt;"", $D2&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>OR($A2&lt;&gt;"", $B2&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C2&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D89"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="3"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="D70" s="4"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="3"/>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="D81" s="4"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:D1">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$A1="group_name"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>OR($A1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", $D1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11694,45 +12879,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="27" priority="2">
+  <conditionalFormatting sqref="A1:F1">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="26" priority="1">
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" dxfId="33" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11743,10 +12935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11756,10 +12948,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -11768,14 +12960,17 @@
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="31" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11789,7 +12984,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11799,13 +12994,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11813,12 +13008,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="30" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11832,7 +13027,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11842,10 +13037,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -11880,12 +13075,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11909,13 +13104,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11932,12 +13127,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11951,7 +13146,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11961,16 +13156,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -11998,12 +13193,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12017,7 +13212,7 @@
   <dimension ref="A1:B602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12027,7 +13222,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12555,12 +13750,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12571,511 +13766,535 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
+      <c r="F1" s="3" t="s">
+        <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="D3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="D5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="4:8">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="4:8">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="4:8">
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="4:8">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="4:8">
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="4:8">
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="4:8">
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="4:8">
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="4:8">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="4:8">
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="4:8">
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="4:8">
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="4:8">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="4:8">
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="4:8">
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="4:8">
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="4:8">
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="4:8">
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="4:8">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="4:8">
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="4:8">
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="4:8">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="4:8">
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="4:8">
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="4:8">
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="4:8">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="4:8">
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="4:8">
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="4:8">
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="4:8">
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="4:8">
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="4:8">
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="4:8">
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="4:8">
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="4:8">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="4:8">
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="2:6">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="4:8">
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="4:8">
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="4:8">
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="2:6">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="4:8">
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="2:6">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="4:8">
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="2:6">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="4:8">
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="2:6">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="4:8">
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="2:6">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="4:8">
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="2:6">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="4:8">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="2:6">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="4:8">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="2:6">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="4:8">
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="2:6">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="4:8">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="2:6">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="4:8">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="2:6">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="4:8">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="2:6">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="4:8">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="2:6">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="4:8">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="2:6">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="4:8">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="2:6">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="4:8">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="2:6">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="4:8">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="2:6">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="4:8">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="13" priority="2">
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+  <conditionalFormatting sqref="A1:I1 A3:I1048576 A2:G2 I2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" dxfId="18" priority="1">
+      <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to inputs sheet check #12
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -24,17 +24,18 @@
     <sheet name="9. specify" sheetId="9" r:id="rId10"/>
     <sheet name="10. dates" sheetId="10" r:id="rId11"/>
     <sheet name="11. outliers" sheetId="11" r:id="rId12"/>
-    <sheet name="enumdb" sheetId="13" r:id="rId13"/>
-    <sheet name="research oneway" sheetId="16" r:id="rId14"/>
-    <sheet name="research twoway" sheetId="17" r:id="rId15"/>
-    <sheet name="text audit" sheetId="19" r:id="rId16"/>
+    <sheet name="12. field comments" sheetId="20" r:id="rId13"/>
+    <sheet name="enumdb" sheetId="13" r:id="rId14"/>
+    <sheet name="research oneway" sheetId="16" r:id="rId15"/>
+    <sheet name="research twoway" sheetId="17" r:id="rId16"/>
+    <sheet name="text audit" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>variable</t>
   </si>
@@ -210,10 +211,13 @@
     <t>group_name</t>
   </si>
   <si>
-    <t>Field Comment</t>
+    <t>Replacements Log (opt.)</t>
   </si>
   <si>
-    <t>Replacements Log (opt.)</t>
+    <t>SurveyCTO Media Folder (opt.)</t>
+  </si>
+  <si>
+    <t>Field Comments</t>
   </si>
 </sst>
 </file>
@@ -544,10 +548,10 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -570,7 +574,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="40">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -722,6 +762,53 @@
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.49995422223578601"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -3315,6 +3402,462 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06BD5AB8-0192-4B56-B181-C4561E1D3603}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2809875" y="47626"/>
+          <a:ext cx="3648075" cy="952499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check # 12</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>Export Field Comments.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check imports, append and output all field comments in in dataset into the HFC output file</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B03C3E77-7AC4-4BBB-9558-3AC9B5F74C96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2809875" y="1104900"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>keep</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D97A6481-1C87-4A59-944D-084FB40E2B18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2809875" y="1781175"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BCDF35-E3F4-4C82-BB86-F9C605F2FCA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7048500" y="361950"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60897BD-C2C0-45BF-9906-CA90719EA899}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{783CBFCB-6768-4171-A8F5-CED9EA3F3757}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A10F9214-9238-498D-AD3D-DB9A86475BC4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -3995,7 +4538,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4663,7 +5206,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5416,7 +5959,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5503,83 +6046,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
             <a:t> command produces a spreadsheet of average time spent on each field and group by enumerator</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D5AABD-5DE5-46C6-9F00-821662E28DB6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4191000" y="1819275"/>
-          <a:ext cx="3667125" cy="638175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>variable</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the name of variables to include for group. Use * for all variables in the group</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5666,15 +6132,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5689,8 +6155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5562600" y="2571749"/>
-          <a:ext cx="3667125" cy="819151"/>
+          <a:off x="5572125" y="1819274"/>
+          <a:ext cx="3667125" cy="762001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5733,13 +6199,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies variables to exclude from group. This column be used to exclude variable when wild cards are used</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>in the variable column </a:t>
+            <a:t>This column specifies variables to exclude from group. By default, all variables in group are included in calculating duration for group</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5944,14 +6404,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5966,7 +6426,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581650" y="3476625"/>
+          <a:off x="5581650" y="3324225"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6013,6 +6473,152 @@
             <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE73667-0845-4F0C-AB6B-C747064E2FEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="2647950"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>keep</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11492,10 +12098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11542,35 +12148,35 @@
       <c r="A6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3">
@@ -11581,153 +12187,157 @@
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="17" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="18"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="12"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="13" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="32" t="s">
-        <v>58</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="17" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="22" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A30" s="18"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="10"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="8"/>
+    <row r="33" spans="1:3">
+      <c r="A33" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="8"/>
@@ -11737,6 +12347,9 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="8"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11752,7 +12365,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11832,12 +12445,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$A1="child"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11851,7 +12464,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11899,17 +12512,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1 A3:G1048576 A2:B2 D2:G2">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11923,7 +12536,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -11980,17 +12593,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1 A3:E1048576 A2:C2 E2">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12000,6 +12613,61 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="27" customFormat="1">
+      <c r="A1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="26"/>
+    </row>
+    <row r="2" spans="1:3" s="27" customFormat="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+    </row>
+    <row r="3" spans="1:3" s="27" customFormat="1">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" spans="1:3" s="27" customFormat="1">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+    </row>
+    <row r="5" spans="1:3" s="27" customFormat="1"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2 A1:B1 A3:B1048576">
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>#REF!&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>#REF!&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="expression" dxfId="12" priority="25">
+      <formula>A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
@@ -12250,12 +12918,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12264,12 +12932,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12440,12 +13108,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12454,12 +13122,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12629,22 +13297,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>$A$1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1 A3:D1048576 D2">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A2&lt;&gt;"", $B2&lt;&gt;"", $C2&lt;&gt;"", $D2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>OR($A2&lt;&gt;"", $B2&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12653,12 +13321,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12668,10 +13336,10 @@
         <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -12690,14 +13358,29 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
+      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3"/>
@@ -12719,7 +13402,26 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
+      <c r="A15" s="3"/>
       <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3"/>
@@ -12741,7 +13443,26 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4">
+      <c r="A26" s="3"/>
       <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3"/>
@@ -12863,13 +13584,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A1="group_name"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="0" priority="19">
-      <formula>OR($A1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", $D1&lt;&gt;"")</formula>
+  <conditionalFormatting sqref="A1:D1 A5:D1048576 B2:D4">
+    <cfRule type="expression" dxfId="2" priority="24">
+      <formula>OR($A1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $D1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A4">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A3&lt;&gt;"", $B3&lt;&gt;"", $D3&lt;&gt;"", $E3&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OR($A2&lt;&gt;"", $B2&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $D2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12882,7 +13613,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12919,12 +13650,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="34" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="33" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12938,7 +13669,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -12965,12 +13696,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="36" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12984,7 +13715,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -13008,12 +13739,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="34" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13027,7 +13758,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -13075,12 +13806,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13094,7 +13825,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -13127,12 +13858,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="30" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13146,7 +13877,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -13193,12 +13924,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13212,7 +13943,7 @@
   <dimension ref="A1:B602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -13750,12 +14481,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13768,8 +14499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -14283,17 +15014,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1 A3:I1048576 A2:G2 I2">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add back check options to input sheet and import command
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherboyer/Dropbox/Github/scratch/high-frequency-checks/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{000A7856-71E8-9A49-B6CE-E0FD3F535D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -27,13 +28,14 @@
     <sheet name="enumdb" sheetId="13" r:id="rId13"/>
     <sheet name="research oneway" sheetId="16" r:id="rId14"/>
     <sheet name="research twoway" sheetId="17" r:id="rId15"/>
+    <sheet name="backchecks" sheetId="18" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>variable</t>
   </si>
@@ -193,12 +195,51 @@
   <si>
     <t>by</t>
   </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>ttest</t>
+  </si>
+  <si>
+    <t>reliability</t>
+  </si>
+  <si>
+    <t>Back Check Dataset</t>
+  </si>
+  <si>
+    <t>Enumerator Team</t>
+  </si>
+  <si>
+    <t>Backchecker ID</t>
+  </si>
+  <si>
+    <t>Backchecker Team</t>
+  </si>
+  <si>
+    <t>okrange_min</t>
+  </si>
+  <si>
+    <t>okrange_max</t>
+  </si>
+  <si>
+    <t>5. Back Check Options</t>
+  </si>
+  <si>
+    <t>Variables to keep from survey</t>
+  </si>
+  <si>
+    <t>Variables to keep from back check</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -241,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -425,11 +466,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -440,9 +490,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -472,6 +519,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -494,7 +546,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1337,7 +1418,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="695325"/>
+          <a:off x="11166475" y="695325"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -2327,7 +2408,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13954125" y="590550"/>
+          <a:off x="15890875" y="590550"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -2946,7 +3027,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="361950"/>
+          <a:off x="11166475" y="361950"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -3630,7 +3711,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12582525" y="495300"/>
+          <a:off x="14325600" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -4221,7 +4302,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8439150" y="495300"/>
+          <a:off x="9601200" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -4754,7 +4835,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9820275" y="495300"/>
+          <a:off x="11176000" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -5670,7 +5751,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11191875" y="314325"/>
+          <a:off x="12741275" y="314325"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -6298,7 +6379,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8429625" y="323850"/>
+          <a:off x="9591675" y="323850"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -6917,7 +6998,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="304800"/>
+          <a:off x="11166475" y="304800"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -7456,7 +7537,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8439150" y="304800"/>
+          <a:off x="9601200" y="304800"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -8020,7 +8101,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="495300"/>
+          <a:off x="11166475" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -8304,7 +8385,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11201400" y="381000"/>
+          <a:off x="12750800" y="381000"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -9259,7 +9340,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7038975" y="600075"/>
+          <a:off x="8007350" y="600075"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -10148,7 +10229,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13954125" y="581025"/>
+          <a:off x="15890875" y="581025"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -10614,224 +10695,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="17" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="13" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="13" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="11"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="22" t="s">
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="13" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="8"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="8"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10843,16 +10973,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -10866,72 +10996,72 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D17" s="3"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$A1="child"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10941,16 +11071,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -10973,19 +11103,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -10993,12 +11123,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11008,16 +11138,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11032,31 +11162,31 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11066,16 +11196,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -11095,13 +11225,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -11109,20 +11239,20 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -11130,11 +11260,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -11142,11 +11272,11 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -11154,11 +11284,11 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -11166,11 +11296,11 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -11178,11 +11308,11 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -11190,11 +11320,11 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -11202,11 +11332,11 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -11214,11 +11344,11 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -11226,11 +11356,11 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -11238,11 +11368,11 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -11250,11 +11380,11 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -11262,11 +11392,11 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -11274,11 +11404,11 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -11286,11 +11416,11 @@
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11300,12 +11430,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11315,16 +11445,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11335,167 +11465,167 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="C70" s="4"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="C81" s="4"/>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", #REF!&lt;&gt;"", $C1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11505,16 +11635,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11528,149 +11658,149 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="4"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D70" s="4"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D81" s="4"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11678,12 +11808,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$A$1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>OR(#REF!&lt;&gt;"", #REF!&lt;&gt;"", $A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11692,20 +11822,114 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A5B874-84EA-A84B-BE56-2FDD54DF9FC8}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="5" width="20.83203125" style="27" customWidth="1"/>
+    <col min="6" max="7" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="E4" s="26"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G1">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$A1="variable"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:G1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11722,16 +11946,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
+    <cfRule type="expression" dxfId="29" priority="2">
+      <formula>$A1="variable"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:E1048576">
+    <cfRule type="expression" dxfId="28" priority="1">
+      <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C1">
     <cfRule type="expression" dxfId="27" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E1048576">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="expression" dxfId="26" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -11741,60 +12008,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="25" priority="2">
-      <formula>$A1="variable"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="24" priority="1">
-      <formula>$A1&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11808,17 +12032,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11828,16 +12052,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11848,63 +12072,64 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11918,26 +12143,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11947,16 +12172,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11973,24 +12198,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -11998,12 +12223,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12013,16 +12238,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12030,537 +12255,537 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="3"/>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="3"/>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" s="3"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="3"/>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B107" s="3"/>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" s="3"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" s="3"/>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" s="3"/>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B137" s="3"/>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B139" s="3"/>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B152" s="3"/>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B154" s="3"/>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B167" s="3"/>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B169" s="3"/>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B182" s="3"/>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B184" s="3"/>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B197" s="3"/>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B199" s="3"/>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B212" s="3"/>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B214" s="3"/>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3"/>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B227" s="3"/>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B229" s="3"/>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B242" s="3"/>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B244" s="3"/>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="3"/>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B257" s="3"/>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B259" s="3"/>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B272" s="3"/>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B274" s="3"/>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B287" s="3"/>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B289" s="3"/>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B302" s="3"/>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B304" s="3"/>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="3"/>
       <c r="B315" s="3"/>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B317" s="3"/>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B319" s="3"/>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="3"/>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B332" s="3"/>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B334" s="3"/>
     </row>
-    <row r="345" spans="1:2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
     </row>
-    <row r="346" spans="1:2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="3"/>
     </row>
-    <row r="347" spans="1:2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B347" s="3"/>
     </row>
-    <row r="349" spans="1:2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B349" s="3"/>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="3"/>
       <c r="B360" s="3"/>
     </row>
-    <row r="361" spans="1:2">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="3"/>
     </row>
-    <row r="362" spans="1:2">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B362" s="3"/>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B364" s="3"/>
     </row>
-    <row r="375" spans="1:2">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="3"/>
       <c r="B375" s="3"/>
     </row>
-    <row r="376" spans="1:2">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="3"/>
     </row>
-    <row r="377" spans="1:2">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B377" s="3"/>
     </row>
-    <row r="379" spans="1:2">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B379" s="3"/>
     </row>
-    <row r="390" spans="1:2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="3"/>
       <c r="B390" s="3"/>
     </row>
-    <row r="391" spans="1:2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="3"/>
     </row>
-    <row r="392" spans="1:2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B392" s="3"/>
     </row>
-    <row r="394" spans="1:2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B394" s="3"/>
     </row>
-    <row r="405" spans="1:2">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="3"/>
       <c r="B405" s="3"/>
     </row>
-    <row r="406" spans="1:2">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="3"/>
     </row>
-    <row r="407" spans="1:2">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B407" s="3"/>
     </row>
-    <row r="409" spans="1:2">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B409" s="3"/>
     </row>
-    <row r="420" spans="1:2">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="3"/>
       <c r="B420" s="3"/>
     </row>
-    <row r="421" spans="1:2">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="3"/>
     </row>
-    <row r="422" spans="1:2">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B422" s="3"/>
     </row>
-    <row r="424" spans="1:2">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B424" s="3"/>
     </row>
-    <row r="435" spans="1:2">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="3"/>
       <c r="B435" s="3"/>
     </row>
-    <row r="436" spans="1:2">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="3"/>
     </row>
-    <row r="437" spans="1:2">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B437" s="3"/>
     </row>
-    <row r="439" spans="1:2">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B439" s="3"/>
     </row>
-    <row r="450" spans="1:2">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="3"/>
       <c r="B450" s="3"/>
     </row>
-    <row r="451" spans="1:2">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="3"/>
     </row>
-    <row r="452" spans="1:2">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B452" s="3"/>
     </row>
-    <row r="454" spans="1:2">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B454" s="3"/>
     </row>
-    <row r="465" spans="1:2">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
     </row>
-    <row r="466" spans="1:2">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="3"/>
     </row>
-    <row r="467" spans="1:2">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B467" s="3"/>
     </row>
-    <row r="469" spans="1:2">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B469" s="3"/>
     </row>
-    <row r="480" spans="1:2">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" s="3"/>
       <c r="B480" s="3"/>
     </row>
-    <row r="481" spans="1:2">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" s="3"/>
     </row>
-    <row r="482" spans="1:2">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B482" s="3"/>
     </row>
-    <row r="484" spans="1:2">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B484" s="3"/>
     </row>
-    <row r="495" spans="1:2">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A495" s="3"/>
       <c r="B495" s="3"/>
     </row>
-    <row r="496" spans="1:2">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" s="3"/>
     </row>
-    <row r="497" spans="1:2">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B497" s="3"/>
     </row>
-    <row r="499" spans="1:2">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B499" s="3"/>
     </row>
-    <row r="510" spans="1:2">
+    <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" s="3"/>
       <c r="B510" s="3"/>
     </row>
-    <row r="511" spans="1:2">
+    <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" s="3"/>
     </row>
-    <row r="512" spans="1:2">
+    <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B512" s="3"/>
     </row>
-    <row r="514" spans="1:2">
+    <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B514" s="3"/>
     </row>
-    <row r="525" spans="1:2">
+    <row r="525" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A525" s="3"/>
       <c r="B525" s="3"/>
     </row>
-    <row r="526" spans="1:2">
+    <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" s="3"/>
     </row>
-    <row r="527" spans="1:2">
+    <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B527" s="3"/>
     </row>
-    <row r="529" spans="1:2">
+    <row r="529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B529" s="3"/>
     </row>
-    <row r="540" spans="1:2">
+    <row r="540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A540" s="3"/>
       <c r="B540" s="3"/>
     </row>
-    <row r="541" spans="1:2">
+    <row r="541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A541" s="3"/>
     </row>
-    <row r="542" spans="1:2">
+    <row r="542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B542" s="3"/>
     </row>
-    <row r="544" spans="1:2">
+    <row r="544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B544" s="3"/>
     </row>
-    <row r="555" spans="1:2">
+    <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" s="3"/>
       <c r="B555" s="3"/>
     </row>
-    <row r="556" spans="1:2">
+    <row r="556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A556" s="3"/>
     </row>
-    <row r="557" spans="1:2">
+    <row r="557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B557" s="3"/>
     </row>
-    <row r="559" spans="1:2">
+    <row r="559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B559" s="3"/>
     </row>
-    <row r="570" spans="1:2">
+    <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
     </row>
-    <row r="571" spans="1:2">
+    <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" s="3"/>
     </row>
-    <row r="572" spans="1:2">
+    <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B572" s="3"/>
     </row>
-    <row r="574" spans="1:2">
+    <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B574" s="3"/>
     </row>
-    <row r="585" spans="1:2">
+    <row r="585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A585" s="3"/>
       <c r="B585" s="3"/>
     </row>
-    <row r="586" spans="1:2">
+    <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" s="3"/>
     </row>
-    <row r="587" spans="1:2">
+    <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B587" s="3"/>
     </row>
-    <row r="589" spans="1:2">
+    <row r="589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B589" s="3"/>
     </row>
-    <row r="600" spans="1:2">
+    <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" s="3"/>
       <c r="B600" s="3"/>
     </row>
-    <row r="601" spans="1:2">
+    <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" s="3"/>
     </row>
-    <row r="602" spans="1:2">
+    <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B602" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12570,16 +12795,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12602,465 +12827,465 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -13069,12 +13294,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Change import and inputs to be logic instead of skip
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs.xlsx
+++ b/xlsx/hfc_inputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherboyer/Dropbox/Github/scratch/high-frequency-checks/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A6C7B-59E3-B34E-8B49-6D3158E9B3B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18320" windowHeight="15420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. setup" sheetId="15" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="3. consent" sheetId="3" r:id="rId4"/>
     <sheet name="4. no miss" sheetId="4" r:id="rId5"/>
     <sheet name="5. follow up" sheetId="5" r:id="rId6"/>
-    <sheet name="6. skip" sheetId="6" r:id="rId7"/>
+    <sheet name="6. logic" sheetId="6" r:id="rId7"/>
     <sheet name="7. all miss" sheetId="7" r:id="rId8"/>
     <sheet name="8. constraints" sheetId="8" r:id="rId9"/>
     <sheet name="9. specify" sheetId="9" r:id="rId10"/>
@@ -28,7 +29,7 @@
     <sheet name="research oneway" sheetId="16" r:id="rId14"/>
     <sheet name="research twoway" sheetId="17" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -197,8 +198,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2946,7 +2947,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="361950"/>
+          <a:off x="11166475" y="361950"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -4754,7 +4755,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9820275" y="495300"/>
+          <a:off x="11176000" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -8304,7 +8305,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11201400" y="381000"/>
+          <a:off x="12750800" y="381000"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -10614,223 +10615,223 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1">
+    <row r="2" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="15"/>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="15"/>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="12"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="15"/>
       <c r="C25" s="11"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="10"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
     </row>
   </sheetData>
@@ -10843,16 +10844,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -10866,60 +10867,60 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D17" s="3"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -10941,16 +10942,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -10973,19 +10974,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -11008,16 +11009,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11032,19 +11033,19 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -11066,16 +11067,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -11095,13 +11096,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -11109,20 +11110,20 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -11130,11 +11131,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -11142,11 +11143,11 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -11154,11 +11155,11 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -11166,11 +11167,11 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -11178,11 +11179,11 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -11190,11 +11191,11 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -11202,11 +11203,11 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -11214,11 +11215,11 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -11226,11 +11227,11 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -11238,11 +11239,11 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -11250,11 +11251,11 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -11262,11 +11263,11 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -11274,11 +11275,11 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -11286,11 +11287,11 @@
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11315,16 +11316,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11335,155 +11336,155 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="C70" s="4"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="C81" s="4"/>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11505,16 +11506,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11528,149 +11529,149 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="4"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D70" s="4"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D81" s="4"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -11693,19 +11694,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11722,7 +11723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11742,16 +11743,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11762,10 +11763,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11785,16 +11786,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11808,7 +11809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
@@ -11828,16 +11829,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11848,34 +11849,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
     </row>
   </sheetData>
@@ -11895,16 +11896,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11918,15 +11919,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
@@ -11947,16 +11948,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -11973,24 +11974,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -12013,16 +12014,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12030,527 +12031,527 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" s="3"/>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="3"/>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="3"/>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" s="3"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="3"/>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B107" s="3"/>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" s="3"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" s="3"/>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" s="3"/>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B137" s="3"/>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B139" s="3"/>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B152" s="3"/>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B154" s="3"/>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B167" s="3"/>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B169" s="3"/>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B182" s="3"/>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B184" s="3"/>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B197" s="3"/>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B199" s="3"/>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="3"/>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B212" s="3"/>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B214" s="3"/>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3"/>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B227" s="3"/>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B229" s="3"/>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="3"/>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B242" s="3"/>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B244" s="3"/>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="3"/>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B257" s="3"/>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B259" s="3"/>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="3"/>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B272" s="3"/>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B274" s="3"/>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B287" s="3"/>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B289" s="3"/>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B302" s="3"/>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B304" s="3"/>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="3"/>
       <c r="B315" s="3"/>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B317" s="3"/>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B319" s="3"/>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="3"/>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B332" s="3"/>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B334" s="3"/>
     </row>
-    <row r="345" spans="1:2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
     </row>
-    <row r="346" spans="1:2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="3"/>
     </row>
-    <row r="347" spans="1:2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B347" s="3"/>
     </row>
-    <row r="349" spans="1:2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B349" s="3"/>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="3"/>
       <c r="B360" s="3"/>
     </row>
-    <row r="361" spans="1:2">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="3"/>
     </row>
-    <row r="362" spans="1:2">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B362" s="3"/>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B364" s="3"/>
     </row>
-    <row r="375" spans="1:2">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="3"/>
       <c r="B375" s="3"/>
     </row>
-    <row r="376" spans="1:2">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="3"/>
     </row>
-    <row r="377" spans="1:2">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B377" s="3"/>
     </row>
-    <row r="379" spans="1:2">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B379" s="3"/>
     </row>
-    <row r="390" spans="1:2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="3"/>
       <c r="B390" s="3"/>
     </row>
-    <row r="391" spans="1:2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="3"/>
     </row>
-    <row r="392" spans="1:2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B392" s="3"/>
     </row>
-    <row r="394" spans="1:2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B394" s="3"/>
     </row>
-    <row r="405" spans="1:2">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="3"/>
       <c r="B405" s="3"/>
     </row>
-    <row r="406" spans="1:2">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="3"/>
     </row>
-    <row r="407" spans="1:2">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B407" s="3"/>
     </row>
-    <row r="409" spans="1:2">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B409" s="3"/>
     </row>
-    <row r="420" spans="1:2">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="3"/>
       <c r="B420" s="3"/>
     </row>
-    <row r="421" spans="1:2">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="3"/>
     </row>
-    <row r="422" spans="1:2">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B422" s="3"/>
     </row>
-    <row r="424" spans="1:2">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B424" s="3"/>
     </row>
-    <row r="435" spans="1:2">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="3"/>
       <c r="B435" s="3"/>
     </row>
-    <row r="436" spans="1:2">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="3"/>
     </row>
-    <row r="437" spans="1:2">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B437" s="3"/>
     </row>
-    <row r="439" spans="1:2">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B439" s="3"/>
     </row>
-    <row r="450" spans="1:2">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="3"/>
       <c r="B450" s="3"/>
     </row>
-    <row r="451" spans="1:2">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="3"/>
     </row>
-    <row r="452" spans="1:2">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B452" s="3"/>
     </row>
-    <row r="454" spans="1:2">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B454" s="3"/>
     </row>
-    <row r="465" spans="1:2">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
     </row>
-    <row r="466" spans="1:2">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="3"/>
     </row>
-    <row r="467" spans="1:2">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B467" s="3"/>
     </row>
-    <row r="469" spans="1:2">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B469" s="3"/>
     </row>
-    <row r="480" spans="1:2">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" s="3"/>
       <c r="B480" s="3"/>
     </row>
-    <row r="481" spans="1:2">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" s="3"/>
     </row>
-    <row r="482" spans="1:2">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B482" s="3"/>
     </row>
-    <row r="484" spans="1:2">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B484" s="3"/>
     </row>
-    <row r="495" spans="1:2">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A495" s="3"/>
       <c r="B495" s="3"/>
     </row>
-    <row r="496" spans="1:2">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" s="3"/>
     </row>
-    <row r="497" spans="1:2">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B497" s="3"/>
     </row>
-    <row r="499" spans="1:2">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B499" s="3"/>
     </row>
-    <row r="510" spans="1:2">
+    <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" s="3"/>
       <c r="B510" s="3"/>
     </row>
-    <row r="511" spans="1:2">
+    <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" s="3"/>
     </row>
-    <row r="512" spans="1:2">
+    <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B512" s="3"/>
     </row>
-    <row r="514" spans="1:2">
+    <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B514" s="3"/>
     </row>
-    <row r="525" spans="1:2">
+    <row r="525" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A525" s="3"/>
       <c r="B525" s="3"/>
     </row>
-    <row r="526" spans="1:2">
+    <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" s="3"/>
     </row>
-    <row r="527" spans="1:2">
+    <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B527" s="3"/>
     </row>
-    <row r="529" spans="1:2">
+    <row r="529" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B529" s="3"/>
     </row>
-    <row r="540" spans="1:2">
+    <row r="540" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A540" s="3"/>
       <c r="B540" s="3"/>
     </row>
-    <row r="541" spans="1:2">
+    <row r="541" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A541" s="3"/>
     </row>
-    <row r="542" spans="1:2">
+    <row r="542" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B542" s="3"/>
     </row>
-    <row r="544" spans="1:2">
+    <row r="544" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B544" s="3"/>
     </row>
-    <row r="555" spans="1:2">
+    <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" s="3"/>
       <c r="B555" s="3"/>
     </row>
-    <row r="556" spans="1:2">
+    <row r="556" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A556" s="3"/>
     </row>
-    <row r="557" spans="1:2">
+    <row r="557" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B557" s="3"/>
     </row>
-    <row r="559" spans="1:2">
+    <row r="559" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B559" s="3"/>
     </row>
-    <row r="570" spans="1:2">
+    <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
     </row>
-    <row r="571" spans="1:2">
+    <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" s="3"/>
     </row>
-    <row r="572" spans="1:2">
+    <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B572" s="3"/>
     </row>
-    <row r="574" spans="1:2">
+    <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B574" s="3"/>
     </row>
-    <row r="585" spans="1:2">
+    <row r="585" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A585" s="3"/>
       <c r="B585" s="3"/>
     </row>
-    <row r="586" spans="1:2">
+    <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" s="3"/>
     </row>
-    <row r="587" spans="1:2">
+    <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B587" s="3"/>
     </row>
-    <row r="589" spans="1:2">
+    <row r="589" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B589" s="3"/>
     </row>
-    <row r="600" spans="1:2">
+    <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" s="3"/>
       <c r="B600" s="3"/>
     </row>
-    <row r="601" spans="1:2">
+    <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" s="3"/>
     </row>
-    <row r="602" spans="1:2">
+    <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B602" s="3"/>
     </row>
   </sheetData>
@@ -12570,16 +12571,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12602,465 +12603,465 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>

</xml_diff>